<commit_message>
atualizacao do grafico do forerunner
</commit_message>
<xml_diff>
--- a/assets/base_dados.xlsx
+++ b/assets/base_dados.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="10">
   <si>
     <t>data</t>
   </si>
@@ -34,7 +34,19 @@
     <t>natura</t>
   </si>
   <si>
+    <t>cor</t>
+  </si>
+  <si>
     <t>amazon</t>
+  </si>
+  <si>
+    <t>cinza pó</t>
+  </si>
+  <si>
+    <t>mercado livre</t>
+  </si>
+  <si>
+    <t>preto</t>
   </si>
 </sst>
 </file>
@@ -44,7 +56,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -57,9 +69,19 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <u/>
+      <sz val="11.0"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <u/>
@@ -82,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -96,6 +118,9 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -105,19 +130,22 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="14" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="20" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -390,7 +418,7 @@
       <c r="C2" s="4">
         <v>56.9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="1"/>
@@ -525,16 +553,16 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="5">
+      <c r="A6" s="6">
         <v>45180.0</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="7">
         <v>0.3819444444444444</v>
       </c>
       <c r="C6" s="4">
         <v>56.9</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="1"/>
@@ -561,10 +589,18 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="6">
+        <v>45181.0</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0.4027777777777778</v>
+      </c>
+      <c r="C7" s="4">
+        <v>56.9</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -589,10 +625,18 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" s="6">
+        <v>45182.0</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0.34375</v>
+      </c>
+      <c r="C8" s="4">
+        <v>56.9</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -617,10 +661,18 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="6">
+        <v>45183.0</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0.4722222222222222</v>
+      </c>
+      <c r="C9" s="8">
+        <v>56.9</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -645,10 +697,18 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="6">
+        <v>45184.0</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0.3715277777777778</v>
+      </c>
+      <c r="C10" s="8">
+        <v>56.9</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -673,10 +733,18 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="A11" s="6">
+        <v>45185.0</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0.7465277777777778</v>
+      </c>
+      <c r="C11" s="8">
+        <v>56.9</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -701,10 +769,18 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12" s="6">
+        <v>45186.0</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.59375</v>
+      </c>
+      <c r="C12" s="8">
+        <v>56.9</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -729,7 +805,9 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="1"/>
+      <c r="A13" s="6">
+        <v>45187.0</v>
+      </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -757,7 +835,9 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="1"/>
+      <c r="A14" s="6">
+        <v>45188.0</v>
+      </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -785,7 +865,9 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="1"/>
+      <c r="A15" s="6">
+        <v>45189.0</v>
+      </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -813,7 +895,9 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="1"/>
+      <c r="A16" s="6">
+        <v>45190.0</v>
+      </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -841,7 +925,9 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="1"/>
+      <c r="A17" s="6">
+        <v>45191.0</v>
+      </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -869,7 +955,9 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="1"/>
+      <c r="A18" s="6">
+        <v>45192.0</v>
+      </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -897,7 +985,9 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="1"/>
+      <c r="A19" s="6">
+        <v>45193.0</v>
+      </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -28393,10 +28483,13 @@
       <c r="Z1000" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D2"/>
+  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.787401575" footer="0.0" header="0.0" left="0.511811024" right="0.511811024" top="0.787401575"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -28411,91 +28504,431 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="10.57"/>
-    <col customWidth="1" min="2" max="26" width="8.71"/>
+    <col customWidth="1" min="2" max="3" width="8.71"/>
+    <col customWidth="1" min="4" max="4" width="14.86"/>
+    <col customWidth="1" min="5" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="9">
+      <c r="A2" s="11">
         <v>45177.0</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="12">
         <v>0.3993055555555556</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="9">
         <v>2399.0</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>5</v>
+      <c r="D2" s="13" t="s">
+        <v>6</v>
       </c>
+      <c r="E2" s="10" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="9">
+      <c r="A3" s="11">
         <v>45178.0</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="12">
         <v>0.4305555555555556</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="9">
         <v>2399.0</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>5</v>
+      <c r="D3" s="9" t="s">
+        <v>6</v>
       </c>
+      <c r="E3" s="10" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="11">
+      <c r="A4" s="14">
         <v>45180.0</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="15">
         <v>0.3819444444444444</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="10">
         <v>2399.0</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>5</v>
+      <c r="D4" s="10" t="s">
+        <v>6</v>
       </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1"/>
-    <row r="6" ht="14.25" customHeight="1"/>
-    <row r="7" ht="14.25" customHeight="1"/>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1"/>
+      <c r="E4" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="14">
+        <v>45181.0</v>
+      </c>
+      <c r="B5" s="15">
+        <v>0.4027777777777778</v>
+      </c>
+      <c r="C5" s="10">
+        <v>2584.0</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" customHeight="1">
+      <c r="A6" s="14">
+        <v>45181.0</v>
+      </c>
+      <c r="B6" s="15">
+        <v>0.4027777777777778</v>
+      </c>
+      <c r="C6" s="10">
+        <v>2231.07</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25" customHeight="1">
+      <c r="A7" s="14">
+        <v>45182.0</v>
+      </c>
+      <c r="B7" s="15">
+        <v>0.34375</v>
+      </c>
+      <c r="C7" s="10">
+        <v>2584.0</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25" customHeight="1">
+      <c r="A8" s="14">
+        <v>45182.0</v>
+      </c>
+      <c r="B8" s="15">
+        <v>0.34375</v>
+      </c>
+      <c r="C8" s="10">
+        <v>2231.07</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25" customHeight="1">
+      <c r="A9" s="14">
+        <v>45183.0</v>
+      </c>
+      <c r="B9" s="15">
+        <v>0.4722222222222222</v>
+      </c>
+      <c r="C9" s="10">
+        <v>2584.0</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="M10" s="14"/>
-    </row>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
+      <c r="A10" s="14">
+        <v>45183.0</v>
+      </c>
+      <c r="B10" s="15">
+        <v>0.4722222222222222</v>
+      </c>
+      <c r="C10" s="10">
+        <v>2468.0</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="16"/>
+    </row>
+    <row r="11" ht="14.25" customHeight="1">
+      <c r="A11" s="14">
+        <v>45184.0</v>
+      </c>
+      <c r="B11" s="15">
+        <v>0.3680555555555556</v>
+      </c>
+      <c r="C11" s="10">
+        <v>2720.0</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25" customHeight="1">
+      <c r="A12" s="14">
+        <v>45184.0</v>
+      </c>
+      <c r="B12" s="15">
+        <v>0.3680555555555556</v>
+      </c>
+      <c r="C12" s="10">
+        <v>2468.0</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25" customHeight="1">
+      <c r="A13" s="14">
+        <v>45184.0</v>
+      </c>
+      <c r="B13" s="15">
+        <v>0.3680555555555556</v>
+      </c>
+      <c r="C13" s="10">
+        <v>2584.0</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25" customHeight="1">
+      <c r="A14" s="14">
+        <v>45185.0</v>
+      </c>
+      <c r="B14" s="15">
+        <v>0.7430555555555556</v>
+      </c>
+      <c r="C14" s="10">
+        <v>3724.0</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25" customHeight="1">
+      <c r="A15" s="14">
+        <v>45185.0</v>
+      </c>
+      <c r="B15" s="15">
+        <v>0.7430555555555556</v>
+      </c>
+      <c r="C15" s="10">
+        <v>2468.0</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" customHeight="1">
+      <c r="A16" s="14">
+        <v>45185.0</v>
+      </c>
+      <c r="B16" s="15">
+        <v>0.7430555555555556</v>
+      </c>
+      <c r="C16" s="10">
+        <v>2584.0</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25" customHeight="1">
+      <c r="A17" s="14">
+        <v>45186.0</v>
+      </c>
+      <c r="B17" s="15">
+        <v>0.5902777777777778</v>
+      </c>
+      <c r="C17" s="10">
+        <v>2818.0</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25" customHeight="1">
+      <c r="A18" s="14">
+        <v>45186.0</v>
+      </c>
+      <c r="B18" s="15">
+        <v>0.5902777777777778</v>
+      </c>
+      <c r="C18" s="10">
+        <v>2468.0</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" customHeight="1">
+      <c r="A19" s="14">
+        <v>45186.0</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25" customHeight="1">
+      <c r="A20" s="14">
+        <v>45187.0</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25" customHeight="1">
+      <c r="A21" s="14">
+        <v>45187.0</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25" customHeight="1">
+      <c r="A22" s="14">
+        <v>45187.0</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25" customHeight="1">
+      <c r="A23" s="14">
+        <v>45188.0</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25" customHeight="1">
+      <c r="A24" s="14">
+        <v>45188.0</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" customHeight="1">
+      <c r="A25" s="14">
+        <v>45188.0</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25" customHeight="1">
+      <c r="A26" s="14">
+        <v>45189.0</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25" customHeight="1">
+      <c r="A27" s="14">
+        <v>45189.0</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25" customHeight="1">
+      <c r="A28" s="14">
+        <v>45189.0</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="29" ht="14.25" customHeight="1"/>
     <row r="30" ht="14.25" customHeight="1"/>
     <row r="31" ht="14.25" customHeight="1"/>
@@ -29469,9 +29902,21 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D2"/>
+    <hyperlink r:id="rId2" ref="D6"/>
+    <hyperlink r:id="rId3" ref="D8"/>
+    <hyperlink r:id="rId4" ref="D10"/>
+    <hyperlink r:id="rId5" ref="D11"/>
+    <hyperlink r:id="rId6" ref="D14"/>
+    <hyperlink r:id="rId7" ref="D17"/>
+    <hyperlink r:id="rId8" ref="D20"/>
+    <hyperlink r:id="rId9" ref="D23"/>
+    <hyperlink r:id="rId10" ref="D26"/>
+  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.787401575" footer="0.0" header="0.0" left="0.511811024" right="0.511811024" top="0.787401575"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
busca automatizada com selenium
</commit_message>
<xml_diff>
--- a/assets/base_dados.xlsx
+++ b/assets/base_dados.xlsx
@@ -5,19 +5,20 @@
   <sheets>
     <sheet state="visible" name="protetor_natura" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="forerunner_255s" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="forerunner_245" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="cf6kuLjH62gycolOtdVoRiho9xYEfQ9dqJbGbUHc2Dk="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="n+kSzENzxxOWtlqoy8gbDXs67oKRgb4fnCWjHNAQokM="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="10">
   <si>
     <t>data</t>
   </si>
@@ -53,8 +54,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="hh:mm"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -104,7 +106,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -146,6 +148,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -159,6 +164,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -808,9 +817,15 @@
       <c r="A13" s="6">
         <v>45187.0</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="B13" s="7">
+        <v>0.4097222222222222</v>
+      </c>
+      <c r="C13" s="8">
+        <v>56.9</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -838,9 +853,15 @@
       <c r="A14" s="6">
         <v>45188.0</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="B14" s="7">
+        <v>0.4965277777777778</v>
+      </c>
+      <c r="C14" s="8">
+        <v>56.9</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -28820,6 +28841,9 @@
       <c r="A19" s="14">
         <v>45186.0</v>
       </c>
+      <c r="B19" s="15">
+        <v>0.5902777777777778</v>
+      </c>
       <c r="C19" s="10">
         <v>0.0</v>
       </c>
@@ -28834,6 +28858,12 @@
       <c r="A20" s="14">
         <v>45187.0</v>
       </c>
+      <c r="B20" s="15">
+        <v>0.4131944444444444</v>
+      </c>
+      <c r="C20" s="10">
+        <v>2818.0</v>
+      </c>
       <c r="D20" s="13" t="s">
         <v>6</v>
       </c>
@@ -28844,6 +28874,12 @@
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="14">
         <v>45187.0</v>
+      </c>
+      <c r="B21" s="15">
+        <v>0.4131944444444444</v>
+      </c>
+      <c r="C21" s="10">
+        <v>2468.0</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>8</v>
@@ -28856,6 +28892,12 @@
       <c r="A22" s="14">
         <v>45187.0</v>
       </c>
+      <c r="B22" s="15">
+        <v>0.4131944444444444</v>
+      </c>
+      <c r="C22" s="10">
+        <v>0.0</v>
+      </c>
       <c r="D22" s="10" t="s">
         <v>6</v>
       </c>
@@ -28866,6 +28908,12 @@
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="14">
         <v>45188.0</v>
+      </c>
+      <c r="B23" s="15">
+        <v>0.4965277777777778</v>
+      </c>
+      <c r="C23" s="10">
+        <v>2818.0</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>6</v>
@@ -28878,6 +28926,12 @@
       <c r="A24" s="14">
         <v>45188.0</v>
       </c>
+      <c r="B24" s="15">
+        <v>0.4965277777777778</v>
+      </c>
+      <c r="C24" s="10">
+        <v>2468.0</v>
+      </c>
       <c r="D24" s="10" t="s">
         <v>8</v>
       </c>
@@ -28888,6 +28942,12 @@
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="14">
         <v>45188.0</v>
+      </c>
+      <c r="B25" s="15">
+        <v>0.4965277777777778</v>
+      </c>
+      <c r="C25" s="10">
+        <v>0.0</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>6</v>
@@ -29919,4 +29979,3107 @@
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId11"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="17">
+        <v>45187.0</v>
+      </c>
+      <c r="B2" s="15">
+        <v>0.4131944444444444</v>
+      </c>
+      <c r="C2" s="10">
+        <v>1910.0</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="17">
+        <v>45188.0</v>
+      </c>
+      <c r="B3" s="15">
+        <v>0.4965277777777778</v>
+      </c>
+      <c r="C3" s="10">
+        <v>2400.0</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="17">
+        <v>45188.0</v>
+      </c>
+      <c r="B4" s="15">
+        <v>0.8680555555555556</v>
+      </c>
+      <c r="C4" s="10">
+        <v>2379.0</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="17">
+        <v>45189.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="17">
+        <v>45190.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="17">
+        <v>45191.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="17">
+        <v>45192.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="17">
+        <v>45193.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="17">
+        <v>45194.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="17">
+        <v>45195.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="17">
+        <v>45196.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="17">
+        <v>45197.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="17">
+        <v>45198.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="17">
+        <v>45199.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="17">
+        <v>45200.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="9"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="9"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="9"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="9"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="9"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="9"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="9"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="9"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="9"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="9"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="9"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="9"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="9"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="9"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="9"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="9"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="9"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="9"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="9"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="9"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="9"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="9"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="9"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="9"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="9"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="9"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="9"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="9"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="9"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="9"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="9"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="9"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="9"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="9"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="9"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="9"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="9"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="9"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="9"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="9"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="9"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="9"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="9"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="9"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="9"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="9"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="9"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="9"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="9"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="9"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="9"/>
+    </row>
+    <row r="68">
+      <c r="A68" s="9"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="9"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="9"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="9"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="9"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="9"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="9"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="9"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="9"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="9"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="9"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="9"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="9"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="9"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="9"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="9"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="9"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="9"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="9"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="9"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="9"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="9"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="9"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="9"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="9"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="9"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="9"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="9"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="9"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="9"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="9"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="9"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="9"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="9"/>
+    </row>
+    <row r="102">
+      <c r="A102" s="9"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="9"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="9"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="9"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="9"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="9"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="9"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="9"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="9"/>
+    </row>
+    <row r="111">
+      <c r="A111" s="9"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="9"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="9"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="9"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="9"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="9"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="9"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="9"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="9"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="9"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="9"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="9"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="9"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="9"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="9"/>
+    </row>
+    <row r="126">
+      <c r="A126" s="9"/>
+    </row>
+    <row r="127">
+      <c r="A127" s="9"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="9"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="9"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="9"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="9"/>
+    </row>
+    <row r="132">
+      <c r="A132" s="9"/>
+    </row>
+    <row r="133">
+      <c r="A133" s="9"/>
+    </row>
+    <row r="134">
+      <c r="A134" s="9"/>
+    </row>
+    <row r="135">
+      <c r="A135" s="9"/>
+    </row>
+    <row r="136">
+      <c r="A136" s="9"/>
+    </row>
+    <row r="137">
+      <c r="A137" s="9"/>
+    </row>
+    <row r="138">
+      <c r="A138" s="9"/>
+    </row>
+    <row r="139">
+      <c r="A139" s="9"/>
+    </row>
+    <row r="140">
+      <c r="A140" s="9"/>
+    </row>
+    <row r="141">
+      <c r="A141" s="9"/>
+    </row>
+    <row r="142">
+      <c r="A142" s="9"/>
+    </row>
+    <row r="143">
+      <c r="A143" s="9"/>
+    </row>
+    <row r="144">
+      <c r="A144" s="9"/>
+    </row>
+    <row r="145">
+      <c r="A145" s="9"/>
+    </row>
+    <row r="146">
+      <c r="A146" s="9"/>
+    </row>
+    <row r="147">
+      <c r="A147" s="9"/>
+    </row>
+    <row r="148">
+      <c r="A148" s="9"/>
+    </row>
+    <row r="149">
+      <c r="A149" s="9"/>
+    </row>
+    <row r="150">
+      <c r="A150" s="9"/>
+    </row>
+    <row r="151">
+      <c r="A151" s="9"/>
+    </row>
+    <row r="152">
+      <c r="A152" s="9"/>
+    </row>
+    <row r="153">
+      <c r="A153" s="9"/>
+    </row>
+    <row r="154">
+      <c r="A154" s="9"/>
+    </row>
+    <row r="155">
+      <c r="A155" s="9"/>
+    </row>
+    <row r="156">
+      <c r="A156" s="9"/>
+    </row>
+    <row r="157">
+      <c r="A157" s="9"/>
+    </row>
+    <row r="158">
+      <c r="A158" s="9"/>
+    </row>
+    <row r="159">
+      <c r="A159" s="9"/>
+    </row>
+    <row r="160">
+      <c r="A160" s="9"/>
+    </row>
+    <row r="161">
+      <c r="A161" s="9"/>
+    </row>
+    <row r="162">
+      <c r="A162" s="9"/>
+    </row>
+    <row r="163">
+      <c r="A163" s="9"/>
+    </row>
+    <row r="164">
+      <c r="A164" s="9"/>
+    </row>
+    <row r="165">
+      <c r="A165" s="9"/>
+    </row>
+    <row r="166">
+      <c r="A166" s="9"/>
+    </row>
+    <row r="167">
+      <c r="A167" s="9"/>
+    </row>
+    <row r="168">
+      <c r="A168" s="9"/>
+    </row>
+    <row r="169">
+      <c r="A169" s="9"/>
+    </row>
+    <row r="170">
+      <c r="A170" s="9"/>
+    </row>
+    <row r="171">
+      <c r="A171" s="9"/>
+    </row>
+    <row r="172">
+      <c r="A172" s="9"/>
+    </row>
+    <row r="173">
+      <c r="A173" s="9"/>
+    </row>
+    <row r="174">
+      <c r="A174" s="9"/>
+    </row>
+    <row r="175">
+      <c r="A175" s="9"/>
+    </row>
+    <row r="176">
+      <c r="A176" s="9"/>
+    </row>
+    <row r="177">
+      <c r="A177" s="9"/>
+    </row>
+    <row r="178">
+      <c r="A178" s="9"/>
+    </row>
+    <row r="179">
+      <c r="A179" s="9"/>
+    </row>
+    <row r="180">
+      <c r="A180" s="9"/>
+    </row>
+    <row r="181">
+      <c r="A181" s="9"/>
+    </row>
+    <row r="182">
+      <c r="A182" s="9"/>
+    </row>
+    <row r="183">
+      <c r="A183" s="9"/>
+    </row>
+    <row r="184">
+      <c r="A184" s="9"/>
+    </row>
+    <row r="185">
+      <c r="A185" s="9"/>
+    </row>
+    <row r="186">
+      <c r="A186" s="9"/>
+    </row>
+    <row r="187">
+      <c r="A187" s="9"/>
+    </row>
+    <row r="188">
+      <c r="A188" s="9"/>
+    </row>
+    <row r="189">
+      <c r="A189" s="9"/>
+    </row>
+    <row r="190">
+      <c r="A190" s="9"/>
+    </row>
+    <row r="191">
+      <c r="A191" s="9"/>
+    </row>
+    <row r="192">
+      <c r="A192" s="9"/>
+    </row>
+    <row r="193">
+      <c r="A193" s="9"/>
+    </row>
+    <row r="194">
+      <c r="A194" s="9"/>
+    </row>
+    <row r="195">
+      <c r="A195" s="9"/>
+    </row>
+    <row r="196">
+      <c r="A196" s="9"/>
+    </row>
+    <row r="197">
+      <c r="A197" s="9"/>
+    </row>
+    <row r="198">
+      <c r="A198" s="9"/>
+    </row>
+    <row r="199">
+      <c r="A199" s="9"/>
+    </row>
+    <row r="200">
+      <c r="A200" s="9"/>
+    </row>
+    <row r="201">
+      <c r="A201" s="9"/>
+    </row>
+    <row r="202">
+      <c r="A202" s="9"/>
+    </row>
+    <row r="203">
+      <c r="A203" s="9"/>
+    </row>
+    <row r="204">
+      <c r="A204" s="9"/>
+    </row>
+    <row r="205">
+      <c r="A205" s="9"/>
+    </row>
+    <row r="206">
+      <c r="A206" s="9"/>
+    </row>
+    <row r="207">
+      <c r="A207" s="9"/>
+    </row>
+    <row r="208">
+      <c r="A208" s="9"/>
+    </row>
+    <row r="209">
+      <c r="A209" s="9"/>
+    </row>
+    <row r="210">
+      <c r="A210" s="9"/>
+    </row>
+    <row r="211">
+      <c r="A211" s="9"/>
+    </row>
+    <row r="212">
+      <c r="A212" s="9"/>
+    </row>
+    <row r="213">
+      <c r="A213" s="9"/>
+    </row>
+    <row r="214">
+      <c r="A214" s="9"/>
+    </row>
+    <row r="215">
+      <c r="A215" s="9"/>
+    </row>
+    <row r="216">
+      <c r="A216" s="9"/>
+    </row>
+    <row r="217">
+      <c r="A217" s="9"/>
+    </row>
+    <row r="218">
+      <c r="A218" s="9"/>
+    </row>
+    <row r="219">
+      <c r="A219" s="9"/>
+    </row>
+    <row r="220">
+      <c r="A220" s="9"/>
+    </row>
+    <row r="221">
+      <c r="A221" s="9"/>
+    </row>
+    <row r="222">
+      <c r="A222" s="9"/>
+    </row>
+    <row r="223">
+      <c r="A223" s="9"/>
+    </row>
+    <row r="224">
+      <c r="A224" s="9"/>
+    </row>
+    <row r="225">
+      <c r="A225" s="9"/>
+    </row>
+    <row r="226">
+      <c r="A226" s="9"/>
+    </row>
+    <row r="227">
+      <c r="A227" s="9"/>
+    </row>
+    <row r="228">
+      <c r="A228" s="9"/>
+    </row>
+    <row r="229">
+      <c r="A229" s="9"/>
+    </row>
+    <row r="230">
+      <c r="A230" s="9"/>
+    </row>
+    <row r="231">
+      <c r="A231" s="9"/>
+    </row>
+    <row r="232">
+      <c r="A232" s="9"/>
+    </row>
+    <row r="233">
+      <c r="A233" s="9"/>
+    </row>
+    <row r="234">
+      <c r="A234" s="9"/>
+    </row>
+    <row r="235">
+      <c r="A235" s="9"/>
+    </row>
+    <row r="236">
+      <c r="A236" s="9"/>
+    </row>
+    <row r="237">
+      <c r="A237" s="9"/>
+    </row>
+    <row r="238">
+      <c r="A238" s="9"/>
+    </row>
+    <row r="239">
+      <c r="A239" s="9"/>
+    </row>
+    <row r="240">
+      <c r="A240" s="9"/>
+    </row>
+    <row r="241">
+      <c r="A241" s="9"/>
+    </row>
+    <row r="242">
+      <c r="A242" s="9"/>
+    </row>
+    <row r="243">
+      <c r="A243" s="9"/>
+    </row>
+    <row r="244">
+      <c r="A244" s="9"/>
+    </row>
+    <row r="245">
+      <c r="A245" s="9"/>
+    </row>
+    <row r="246">
+      <c r="A246" s="9"/>
+    </row>
+    <row r="247">
+      <c r="A247" s="9"/>
+    </row>
+    <row r="248">
+      <c r="A248" s="9"/>
+    </row>
+    <row r="249">
+      <c r="A249" s="9"/>
+    </row>
+    <row r="250">
+      <c r="A250" s="9"/>
+    </row>
+    <row r="251">
+      <c r="A251" s="9"/>
+    </row>
+    <row r="252">
+      <c r="A252" s="9"/>
+    </row>
+    <row r="253">
+      <c r="A253" s="9"/>
+    </row>
+    <row r="254">
+      <c r="A254" s="9"/>
+    </row>
+    <row r="255">
+      <c r="A255" s="9"/>
+    </row>
+    <row r="256">
+      <c r="A256" s="9"/>
+    </row>
+    <row r="257">
+      <c r="A257" s="9"/>
+    </row>
+    <row r="258">
+      <c r="A258" s="9"/>
+    </row>
+    <row r="259">
+      <c r="A259" s="9"/>
+    </row>
+    <row r="260">
+      <c r="A260" s="9"/>
+    </row>
+    <row r="261">
+      <c r="A261" s="9"/>
+    </row>
+    <row r="262">
+      <c r="A262" s="9"/>
+    </row>
+    <row r="263">
+      <c r="A263" s="9"/>
+    </row>
+    <row r="264">
+      <c r="A264" s="9"/>
+    </row>
+    <row r="265">
+      <c r="A265" s="9"/>
+    </row>
+    <row r="266">
+      <c r="A266" s="9"/>
+    </row>
+    <row r="267">
+      <c r="A267" s="9"/>
+    </row>
+    <row r="268">
+      <c r="A268" s="9"/>
+    </row>
+    <row r="269">
+      <c r="A269" s="9"/>
+    </row>
+    <row r="270">
+      <c r="A270" s="9"/>
+    </row>
+    <row r="271">
+      <c r="A271" s="9"/>
+    </row>
+    <row r="272">
+      <c r="A272" s="9"/>
+    </row>
+    <row r="273">
+      <c r="A273" s="9"/>
+    </row>
+    <row r="274">
+      <c r="A274" s="9"/>
+    </row>
+    <row r="275">
+      <c r="A275" s="9"/>
+    </row>
+    <row r="276">
+      <c r="A276" s="9"/>
+    </row>
+    <row r="277">
+      <c r="A277" s="9"/>
+    </row>
+    <row r="278">
+      <c r="A278" s="9"/>
+    </row>
+    <row r="279">
+      <c r="A279" s="9"/>
+    </row>
+    <row r="280">
+      <c r="A280" s="9"/>
+    </row>
+    <row r="281">
+      <c r="A281" s="9"/>
+    </row>
+    <row r="282">
+      <c r="A282" s="9"/>
+    </row>
+    <row r="283">
+      <c r="A283" s="9"/>
+    </row>
+    <row r="284">
+      <c r="A284" s="9"/>
+    </row>
+    <row r="285">
+      <c r="A285" s="9"/>
+    </row>
+    <row r="286">
+      <c r="A286" s="9"/>
+    </row>
+    <row r="287">
+      <c r="A287" s="9"/>
+    </row>
+    <row r="288">
+      <c r="A288" s="9"/>
+    </row>
+    <row r="289">
+      <c r="A289" s="9"/>
+    </row>
+    <row r="290">
+      <c r="A290" s="9"/>
+    </row>
+    <row r="291">
+      <c r="A291" s="9"/>
+    </row>
+    <row r="292">
+      <c r="A292" s="9"/>
+    </row>
+    <row r="293">
+      <c r="A293" s="9"/>
+    </row>
+    <row r="294">
+      <c r="A294" s="9"/>
+    </row>
+    <row r="295">
+      <c r="A295" s="9"/>
+    </row>
+    <row r="296">
+      <c r="A296" s="9"/>
+    </row>
+    <row r="297">
+      <c r="A297" s="9"/>
+    </row>
+    <row r="298">
+      <c r="A298" s="9"/>
+    </row>
+    <row r="299">
+      <c r="A299" s="9"/>
+    </row>
+    <row r="300">
+      <c r="A300" s="9"/>
+    </row>
+    <row r="301">
+      <c r="A301" s="9"/>
+    </row>
+    <row r="302">
+      <c r="A302" s="9"/>
+    </row>
+    <row r="303">
+      <c r="A303" s="9"/>
+    </row>
+    <row r="304">
+      <c r="A304" s="9"/>
+    </row>
+    <row r="305">
+      <c r="A305" s="9"/>
+    </row>
+    <row r="306">
+      <c r="A306" s="9"/>
+    </row>
+    <row r="307">
+      <c r="A307" s="9"/>
+    </row>
+    <row r="308">
+      <c r="A308" s="9"/>
+    </row>
+    <row r="309">
+      <c r="A309" s="9"/>
+    </row>
+    <row r="310">
+      <c r="A310" s="9"/>
+    </row>
+    <row r="311">
+      <c r="A311" s="9"/>
+    </row>
+    <row r="312">
+      <c r="A312" s="9"/>
+    </row>
+    <row r="313">
+      <c r="A313" s="9"/>
+    </row>
+    <row r="314">
+      <c r="A314" s="9"/>
+    </row>
+    <row r="315">
+      <c r="A315" s="9"/>
+    </row>
+    <row r="316">
+      <c r="A316" s="9"/>
+    </row>
+    <row r="317">
+      <c r="A317" s="9"/>
+    </row>
+    <row r="318">
+      <c r="A318" s="9"/>
+    </row>
+    <row r="319">
+      <c r="A319" s="9"/>
+    </row>
+    <row r="320">
+      <c r="A320" s="9"/>
+    </row>
+    <row r="321">
+      <c r="A321" s="9"/>
+    </row>
+    <row r="322">
+      <c r="A322" s="9"/>
+    </row>
+    <row r="323">
+      <c r="A323" s="9"/>
+    </row>
+    <row r="324">
+      <c r="A324" s="9"/>
+    </row>
+    <row r="325">
+      <c r="A325" s="9"/>
+    </row>
+    <row r="326">
+      <c r="A326" s="9"/>
+    </row>
+    <row r="327">
+      <c r="A327" s="9"/>
+    </row>
+    <row r="328">
+      <c r="A328" s="9"/>
+    </row>
+    <row r="329">
+      <c r="A329" s="9"/>
+    </row>
+    <row r="330">
+      <c r="A330" s="9"/>
+    </row>
+    <row r="331">
+      <c r="A331" s="9"/>
+    </row>
+    <row r="332">
+      <c r="A332" s="9"/>
+    </row>
+    <row r="333">
+      <c r="A333" s="9"/>
+    </row>
+    <row r="334">
+      <c r="A334" s="9"/>
+    </row>
+    <row r="335">
+      <c r="A335" s="9"/>
+    </row>
+    <row r="336">
+      <c r="A336" s="9"/>
+    </row>
+    <row r="337">
+      <c r="A337" s="9"/>
+    </row>
+    <row r="338">
+      <c r="A338" s="9"/>
+    </row>
+    <row r="339">
+      <c r="A339" s="9"/>
+    </row>
+    <row r="340">
+      <c r="A340" s="9"/>
+    </row>
+    <row r="341">
+      <c r="A341" s="9"/>
+    </row>
+    <row r="342">
+      <c r="A342" s="9"/>
+    </row>
+    <row r="343">
+      <c r="A343" s="9"/>
+    </row>
+    <row r="344">
+      <c r="A344" s="9"/>
+    </row>
+    <row r="345">
+      <c r="A345" s="9"/>
+    </row>
+    <row r="346">
+      <c r="A346" s="9"/>
+    </row>
+    <row r="347">
+      <c r="A347" s="9"/>
+    </row>
+    <row r="348">
+      <c r="A348" s="9"/>
+    </row>
+    <row r="349">
+      <c r="A349" s="9"/>
+    </row>
+    <row r="350">
+      <c r="A350" s="9"/>
+    </row>
+    <row r="351">
+      <c r="A351" s="9"/>
+    </row>
+    <row r="352">
+      <c r="A352" s="9"/>
+    </row>
+    <row r="353">
+      <c r="A353" s="9"/>
+    </row>
+    <row r="354">
+      <c r="A354" s="9"/>
+    </row>
+    <row r="355">
+      <c r="A355" s="9"/>
+    </row>
+    <row r="356">
+      <c r="A356" s="9"/>
+    </row>
+    <row r="357">
+      <c r="A357" s="9"/>
+    </row>
+    <row r="358">
+      <c r="A358" s="9"/>
+    </row>
+    <row r="359">
+      <c r="A359" s="9"/>
+    </row>
+    <row r="360">
+      <c r="A360" s="9"/>
+    </row>
+    <row r="361">
+      <c r="A361" s="9"/>
+    </row>
+    <row r="362">
+      <c r="A362" s="9"/>
+    </row>
+    <row r="363">
+      <c r="A363" s="9"/>
+    </row>
+    <row r="364">
+      <c r="A364" s="9"/>
+    </row>
+    <row r="365">
+      <c r="A365" s="9"/>
+    </row>
+    <row r="366">
+      <c r="A366" s="9"/>
+    </row>
+    <row r="367">
+      <c r="A367" s="9"/>
+    </row>
+    <row r="368">
+      <c r="A368" s="9"/>
+    </row>
+    <row r="369">
+      <c r="A369" s="9"/>
+    </row>
+    <row r="370">
+      <c r="A370" s="9"/>
+    </row>
+    <row r="371">
+      <c r="A371" s="9"/>
+    </row>
+    <row r="372">
+      <c r="A372" s="9"/>
+    </row>
+    <row r="373">
+      <c r="A373" s="9"/>
+    </row>
+    <row r="374">
+      <c r="A374" s="9"/>
+    </row>
+    <row r="375">
+      <c r="A375" s="9"/>
+    </row>
+    <row r="376">
+      <c r="A376" s="9"/>
+    </row>
+    <row r="377">
+      <c r="A377" s="9"/>
+    </row>
+    <row r="378">
+      <c r="A378" s="9"/>
+    </row>
+    <row r="379">
+      <c r="A379" s="9"/>
+    </row>
+    <row r="380">
+      <c r="A380" s="9"/>
+    </row>
+    <row r="381">
+      <c r="A381" s="9"/>
+    </row>
+    <row r="382">
+      <c r="A382" s="9"/>
+    </row>
+    <row r="383">
+      <c r="A383" s="9"/>
+    </row>
+    <row r="384">
+      <c r="A384" s="9"/>
+    </row>
+    <row r="385">
+      <c r="A385" s="9"/>
+    </row>
+    <row r="386">
+      <c r="A386" s="9"/>
+    </row>
+    <row r="387">
+      <c r="A387" s="9"/>
+    </row>
+    <row r="388">
+      <c r="A388" s="9"/>
+    </row>
+    <row r="389">
+      <c r="A389" s="9"/>
+    </row>
+    <row r="390">
+      <c r="A390" s="9"/>
+    </row>
+    <row r="391">
+      <c r="A391" s="9"/>
+    </row>
+    <row r="392">
+      <c r="A392" s="9"/>
+    </row>
+    <row r="393">
+      <c r="A393" s="9"/>
+    </row>
+    <row r="394">
+      <c r="A394" s="9"/>
+    </row>
+    <row r="395">
+      <c r="A395" s="9"/>
+    </row>
+    <row r="396">
+      <c r="A396" s="9"/>
+    </row>
+    <row r="397">
+      <c r="A397" s="9"/>
+    </row>
+    <row r="398">
+      <c r="A398" s="9"/>
+    </row>
+    <row r="399">
+      <c r="A399" s="9"/>
+    </row>
+    <row r="400">
+      <c r="A400" s="9"/>
+    </row>
+    <row r="401">
+      <c r="A401" s="9"/>
+    </row>
+    <row r="402">
+      <c r="A402" s="9"/>
+    </row>
+    <row r="403">
+      <c r="A403" s="9"/>
+    </row>
+    <row r="404">
+      <c r="A404" s="9"/>
+    </row>
+    <row r="405">
+      <c r="A405" s="9"/>
+    </row>
+    <row r="406">
+      <c r="A406" s="9"/>
+    </row>
+    <row r="407">
+      <c r="A407" s="9"/>
+    </row>
+    <row r="408">
+      <c r="A408" s="9"/>
+    </row>
+    <row r="409">
+      <c r="A409" s="9"/>
+    </row>
+    <row r="410">
+      <c r="A410" s="9"/>
+    </row>
+    <row r="411">
+      <c r="A411" s="9"/>
+    </row>
+    <row r="412">
+      <c r="A412" s="9"/>
+    </row>
+    <row r="413">
+      <c r="A413" s="9"/>
+    </row>
+    <row r="414">
+      <c r="A414" s="9"/>
+    </row>
+    <row r="415">
+      <c r="A415" s="9"/>
+    </row>
+    <row r="416">
+      <c r="A416" s="9"/>
+    </row>
+    <row r="417">
+      <c r="A417" s="9"/>
+    </row>
+    <row r="418">
+      <c r="A418" s="9"/>
+    </row>
+    <row r="419">
+      <c r="A419" s="9"/>
+    </row>
+    <row r="420">
+      <c r="A420" s="9"/>
+    </row>
+    <row r="421">
+      <c r="A421" s="9"/>
+    </row>
+    <row r="422">
+      <c r="A422" s="9"/>
+    </row>
+    <row r="423">
+      <c r="A423" s="9"/>
+    </row>
+    <row r="424">
+      <c r="A424" s="9"/>
+    </row>
+    <row r="425">
+      <c r="A425" s="9"/>
+    </row>
+    <row r="426">
+      <c r="A426" s="9"/>
+    </row>
+    <row r="427">
+      <c r="A427" s="9"/>
+    </row>
+    <row r="428">
+      <c r="A428" s="9"/>
+    </row>
+    <row r="429">
+      <c r="A429" s="9"/>
+    </row>
+    <row r="430">
+      <c r="A430" s="9"/>
+    </row>
+    <row r="431">
+      <c r="A431" s="9"/>
+    </row>
+    <row r="432">
+      <c r="A432" s="9"/>
+    </row>
+    <row r="433">
+      <c r="A433" s="9"/>
+    </row>
+    <row r="434">
+      <c r="A434" s="9"/>
+    </row>
+    <row r="435">
+      <c r="A435" s="9"/>
+    </row>
+    <row r="436">
+      <c r="A436" s="9"/>
+    </row>
+    <row r="437">
+      <c r="A437" s="9"/>
+    </row>
+    <row r="438">
+      <c r="A438" s="9"/>
+    </row>
+    <row r="439">
+      <c r="A439" s="9"/>
+    </row>
+    <row r="440">
+      <c r="A440" s="9"/>
+    </row>
+    <row r="441">
+      <c r="A441" s="9"/>
+    </row>
+    <row r="442">
+      <c r="A442" s="9"/>
+    </row>
+    <row r="443">
+      <c r="A443" s="9"/>
+    </row>
+    <row r="444">
+      <c r="A444" s="9"/>
+    </row>
+    <row r="445">
+      <c r="A445" s="9"/>
+    </row>
+    <row r="446">
+      <c r="A446" s="9"/>
+    </row>
+    <row r="447">
+      <c r="A447" s="9"/>
+    </row>
+    <row r="448">
+      <c r="A448" s="9"/>
+    </row>
+    <row r="449">
+      <c r="A449" s="9"/>
+    </row>
+    <row r="450">
+      <c r="A450" s="9"/>
+    </row>
+    <row r="451">
+      <c r="A451" s="9"/>
+    </row>
+    <row r="452">
+      <c r="A452" s="9"/>
+    </row>
+    <row r="453">
+      <c r="A453" s="9"/>
+    </row>
+    <row r="454">
+      <c r="A454" s="9"/>
+    </row>
+    <row r="455">
+      <c r="A455" s="9"/>
+    </row>
+    <row r="456">
+      <c r="A456" s="9"/>
+    </row>
+    <row r="457">
+      <c r="A457" s="9"/>
+    </row>
+    <row r="458">
+      <c r="A458" s="9"/>
+    </row>
+    <row r="459">
+      <c r="A459" s="9"/>
+    </row>
+    <row r="460">
+      <c r="A460" s="9"/>
+    </row>
+    <row r="461">
+      <c r="A461" s="9"/>
+    </row>
+    <row r="462">
+      <c r="A462" s="9"/>
+    </row>
+    <row r="463">
+      <c r="A463" s="9"/>
+    </row>
+    <row r="464">
+      <c r="A464" s="9"/>
+    </row>
+    <row r="465">
+      <c r="A465" s="9"/>
+    </row>
+    <row r="466">
+      <c r="A466" s="9"/>
+    </row>
+    <row r="467">
+      <c r="A467" s="9"/>
+    </row>
+    <row r="468">
+      <c r="A468" s="9"/>
+    </row>
+    <row r="469">
+      <c r="A469" s="9"/>
+    </row>
+    <row r="470">
+      <c r="A470" s="9"/>
+    </row>
+    <row r="471">
+      <c r="A471" s="9"/>
+    </row>
+    <row r="472">
+      <c r="A472" s="9"/>
+    </row>
+    <row r="473">
+      <c r="A473" s="9"/>
+    </row>
+    <row r="474">
+      <c r="A474" s="9"/>
+    </row>
+    <row r="475">
+      <c r="A475" s="9"/>
+    </row>
+    <row r="476">
+      <c r="A476" s="9"/>
+    </row>
+    <row r="477">
+      <c r="A477" s="9"/>
+    </row>
+    <row r="478">
+      <c r="A478" s="9"/>
+    </row>
+    <row r="479">
+      <c r="A479" s="9"/>
+    </row>
+    <row r="480">
+      <c r="A480" s="9"/>
+    </row>
+    <row r="481">
+      <c r="A481" s="9"/>
+    </row>
+    <row r="482">
+      <c r="A482" s="9"/>
+    </row>
+    <row r="483">
+      <c r="A483" s="9"/>
+    </row>
+    <row r="484">
+      <c r="A484" s="9"/>
+    </row>
+    <row r="485">
+      <c r="A485" s="9"/>
+    </row>
+    <row r="486">
+      <c r="A486" s="9"/>
+    </row>
+    <row r="487">
+      <c r="A487" s="9"/>
+    </row>
+    <row r="488">
+      <c r="A488" s="9"/>
+    </row>
+    <row r="489">
+      <c r="A489" s="9"/>
+    </row>
+    <row r="490">
+      <c r="A490" s="9"/>
+    </row>
+    <row r="491">
+      <c r="A491" s="9"/>
+    </row>
+    <row r="492">
+      <c r="A492" s="9"/>
+    </row>
+    <row r="493">
+      <c r="A493" s="9"/>
+    </row>
+    <row r="494">
+      <c r="A494" s="9"/>
+    </row>
+    <row r="495">
+      <c r="A495" s="9"/>
+    </row>
+    <row r="496">
+      <c r="A496" s="9"/>
+    </row>
+    <row r="497">
+      <c r="A497" s="9"/>
+    </row>
+    <row r="498">
+      <c r="A498" s="9"/>
+    </row>
+    <row r="499">
+      <c r="A499" s="9"/>
+    </row>
+    <row r="500">
+      <c r="A500" s="9"/>
+    </row>
+    <row r="501">
+      <c r="A501" s="9"/>
+    </row>
+    <row r="502">
+      <c r="A502" s="9"/>
+    </row>
+    <row r="503">
+      <c r="A503" s="9"/>
+    </row>
+    <row r="504">
+      <c r="A504" s="9"/>
+    </row>
+    <row r="505">
+      <c r="A505" s="9"/>
+    </row>
+    <row r="506">
+      <c r="A506" s="9"/>
+    </row>
+    <row r="507">
+      <c r="A507" s="9"/>
+    </row>
+    <row r="508">
+      <c r="A508" s="9"/>
+    </row>
+    <row r="509">
+      <c r="A509" s="9"/>
+    </row>
+    <row r="510">
+      <c r="A510" s="9"/>
+    </row>
+    <row r="511">
+      <c r="A511" s="9"/>
+    </row>
+    <row r="512">
+      <c r="A512" s="9"/>
+    </row>
+    <row r="513">
+      <c r="A513" s="9"/>
+    </row>
+    <row r="514">
+      <c r="A514" s="9"/>
+    </row>
+    <row r="515">
+      <c r="A515" s="9"/>
+    </row>
+    <row r="516">
+      <c r="A516" s="9"/>
+    </row>
+    <row r="517">
+      <c r="A517" s="9"/>
+    </row>
+    <row r="518">
+      <c r="A518" s="9"/>
+    </row>
+    <row r="519">
+      <c r="A519" s="9"/>
+    </row>
+    <row r="520">
+      <c r="A520" s="9"/>
+    </row>
+    <row r="521">
+      <c r="A521" s="9"/>
+    </row>
+    <row r="522">
+      <c r="A522" s="9"/>
+    </row>
+    <row r="523">
+      <c r="A523" s="9"/>
+    </row>
+    <row r="524">
+      <c r="A524" s="9"/>
+    </row>
+    <row r="525">
+      <c r="A525" s="9"/>
+    </row>
+    <row r="526">
+      <c r="A526" s="9"/>
+    </row>
+    <row r="527">
+      <c r="A527" s="9"/>
+    </row>
+    <row r="528">
+      <c r="A528" s="9"/>
+    </row>
+    <row r="529">
+      <c r="A529" s="9"/>
+    </row>
+    <row r="530">
+      <c r="A530" s="9"/>
+    </row>
+    <row r="531">
+      <c r="A531" s="9"/>
+    </row>
+    <row r="532">
+      <c r="A532" s="9"/>
+    </row>
+    <row r="533">
+      <c r="A533" s="9"/>
+    </row>
+    <row r="534">
+      <c r="A534" s="9"/>
+    </row>
+    <row r="535">
+      <c r="A535" s="9"/>
+    </row>
+    <row r="536">
+      <c r="A536" s="9"/>
+    </row>
+    <row r="537">
+      <c r="A537" s="9"/>
+    </row>
+    <row r="538">
+      <c r="A538" s="9"/>
+    </row>
+    <row r="539">
+      <c r="A539" s="9"/>
+    </row>
+    <row r="540">
+      <c r="A540" s="9"/>
+    </row>
+    <row r="541">
+      <c r="A541" s="9"/>
+    </row>
+    <row r="542">
+      <c r="A542" s="9"/>
+    </row>
+    <row r="543">
+      <c r="A543" s="9"/>
+    </row>
+    <row r="544">
+      <c r="A544" s="9"/>
+    </row>
+    <row r="545">
+      <c r="A545" s="9"/>
+    </row>
+    <row r="546">
+      <c r="A546" s="9"/>
+    </row>
+    <row r="547">
+      <c r="A547" s="9"/>
+    </row>
+    <row r="548">
+      <c r="A548" s="9"/>
+    </row>
+    <row r="549">
+      <c r="A549" s="9"/>
+    </row>
+    <row r="550">
+      <c r="A550" s="9"/>
+    </row>
+    <row r="551">
+      <c r="A551" s="9"/>
+    </row>
+    <row r="552">
+      <c r="A552" s="9"/>
+    </row>
+    <row r="553">
+      <c r="A553" s="9"/>
+    </row>
+    <row r="554">
+      <c r="A554" s="9"/>
+    </row>
+    <row r="555">
+      <c r="A555" s="9"/>
+    </row>
+    <row r="556">
+      <c r="A556" s="9"/>
+    </row>
+    <row r="557">
+      <c r="A557" s="9"/>
+    </row>
+    <row r="558">
+      <c r="A558" s="9"/>
+    </row>
+    <row r="559">
+      <c r="A559" s="9"/>
+    </row>
+    <row r="560">
+      <c r="A560" s="9"/>
+    </row>
+    <row r="561">
+      <c r="A561" s="9"/>
+    </row>
+    <row r="562">
+      <c r="A562" s="9"/>
+    </row>
+    <row r="563">
+      <c r="A563" s="9"/>
+    </row>
+    <row r="564">
+      <c r="A564" s="9"/>
+    </row>
+    <row r="565">
+      <c r="A565" s="9"/>
+    </row>
+    <row r="566">
+      <c r="A566" s="9"/>
+    </row>
+    <row r="567">
+      <c r="A567" s="9"/>
+    </row>
+    <row r="568">
+      <c r="A568" s="9"/>
+    </row>
+    <row r="569">
+      <c r="A569" s="9"/>
+    </row>
+    <row r="570">
+      <c r="A570" s="9"/>
+    </row>
+    <row r="571">
+      <c r="A571" s="9"/>
+    </row>
+    <row r="572">
+      <c r="A572" s="9"/>
+    </row>
+    <row r="573">
+      <c r="A573" s="9"/>
+    </row>
+    <row r="574">
+      <c r="A574" s="9"/>
+    </row>
+    <row r="575">
+      <c r="A575" s="9"/>
+    </row>
+    <row r="576">
+      <c r="A576" s="9"/>
+    </row>
+    <row r="577">
+      <c r="A577" s="9"/>
+    </row>
+    <row r="578">
+      <c r="A578" s="9"/>
+    </row>
+    <row r="579">
+      <c r="A579" s="9"/>
+    </row>
+    <row r="580">
+      <c r="A580" s="9"/>
+    </row>
+    <row r="581">
+      <c r="A581" s="9"/>
+    </row>
+    <row r="582">
+      <c r="A582" s="9"/>
+    </row>
+    <row r="583">
+      <c r="A583" s="9"/>
+    </row>
+    <row r="584">
+      <c r="A584" s="9"/>
+    </row>
+    <row r="585">
+      <c r="A585" s="9"/>
+    </row>
+    <row r="586">
+      <c r="A586" s="9"/>
+    </row>
+    <row r="587">
+      <c r="A587" s="9"/>
+    </row>
+    <row r="588">
+      <c r="A588" s="9"/>
+    </row>
+    <row r="589">
+      <c r="A589" s="9"/>
+    </row>
+    <row r="590">
+      <c r="A590" s="9"/>
+    </row>
+    <row r="591">
+      <c r="A591" s="9"/>
+    </row>
+    <row r="592">
+      <c r="A592" s="9"/>
+    </row>
+    <row r="593">
+      <c r="A593" s="9"/>
+    </row>
+    <row r="594">
+      <c r="A594" s="9"/>
+    </row>
+    <row r="595">
+      <c r="A595" s="9"/>
+    </row>
+    <row r="596">
+      <c r="A596" s="9"/>
+    </row>
+    <row r="597">
+      <c r="A597" s="9"/>
+    </row>
+    <row r="598">
+      <c r="A598" s="9"/>
+    </row>
+    <row r="599">
+      <c r="A599" s="9"/>
+    </row>
+    <row r="600">
+      <c r="A600" s="9"/>
+    </row>
+    <row r="601">
+      <c r="A601" s="9"/>
+    </row>
+    <row r="602">
+      <c r="A602" s="9"/>
+    </row>
+    <row r="603">
+      <c r="A603" s="9"/>
+    </row>
+    <row r="604">
+      <c r="A604" s="9"/>
+    </row>
+    <row r="605">
+      <c r="A605" s="9"/>
+    </row>
+    <row r="606">
+      <c r="A606" s="9"/>
+    </row>
+    <row r="607">
+      <c r="A607" s="9"/>
+    </row>
+    <row r="608">
+      <c r="A608" s="9"/>
+    </row>
+    <row r="609">
+      <c r="A609" s="9"/>
+    </row>
+    <row r="610">
+      <c r="A610" s="9"/>
+    </row>
+    <row r="611">
+      <c r="A611" s="9"/>
+    </row>
+    <row r="612">
+      <c r="A612" s="9"/>
+    </row>
+    <row r="613">
+      <c r="A613" s="9"/>
+    </row>
+    <row r="614">
+      <c r="A614" s="9"/>
+    </row>
+    <row r="615">
+      <c r="A615" s="9"/>
+    </row>
+    <row r="616">
+      <c r="A616" s="9"/>
+    </row>
+    <row r="617">
+      <c r="A617" s="9"/>
+    </row>
+    <row r="618">
+      <c r="A618" s="9"/>
+    </row>
+    <row r="619">
+      <c r="A619" s="9"/>
+    </row>
+    <row r="620">
+      <c r="A620" s="9"/>
+    </row>
+    <row r="621">
+      <c r="A621" s="9"/>
+    </row>
+    <row r="622">
+      <c r="A622" s="9"/>
+    </row>
+    <row r="623">
+      <c r="A623" s="9"/>
+    </row>
+    <row r="624">
+      <c r="A624" s="9"/>
+    </row>
+    <row r="625">
+      <c r="A625" s="9"/>
+    </row>
+    <row r="626">
+      <c r="A626" s="9"/>
+    </row>
+    <row r="627">
+      <c r="A627" s="9"/>
+    </row>
+    <row r="628">
+      <c r="A628" s="9"/>
+    </row>
+    <row r="629">
+      <c r="A629" s="9"/>
+    </row>
+    <row r="630">
+      <c r="A630" s="9"/>
+    </row>
+    <row r="631">
+      <c r="A631" s="9"/>
+    </row>
+    <row r="632">
+      <c r="A632" s="9"/>
+    </row>
+    <row r="633">
+      <c r="A633" s="9"/>
+    </row>
+    <row r="634">
+      <c r="A634" s="9"/>
+    </row>
+    <row r="635">
+      <c r="A635" s="9"/>
+    </row>
+    <row r="636">
+      <c r="A636" s="9"/>
+    </row>
+    <row r="637">
+      <c r="A637" s="9"/>
+    </row>
+    <row r="638">
+      <c r="A638" s="9"/>
+    </row>
+    <row r="639">
+      <c r="A639" s="9"/>
+    </row>
+    <row r="640">
+      <c r="A640" s="9"/>
+    </row>
+    <row r="641">
+      <c r="A641" s="9"/>
+    </row>
+    <row r="642">
+      <c r="A642" s="9"/>
+    </row>
+    <row r="643">
+      <c r="A643" s="9"/>
+    </row>
+    <row r="644">
+      <c r="A644" s="9"/>
+    </row>
+    <row r="645">
+      <c r="A645" s="9"/>
+    </row>
+    <row r="646">
+      <c r="A646" s="9"/>
+    </row>
+    <row r="647">
+      <c r="A647" s="9"/>
+    </row>
+    <row r="648">
+      <c r="A648" s="9"/>
+    </row>
+    <row r="649">
+      <c r="A649" s="9"/>
+    </row>
+    <row r="650">
+      <c r="A650" s="9"/>
+    </row>
+    <row r="651">
+      <c r="A651" s="9"/>
+    </row>
+    <row r="652">
+      <c r="A652" s="9"/>
+    </row>
+    <row r="653">
+      <c r="A653" s="9"/>
+    </row>
+    <row r="654">
+      <c r="A654" s="9"/>
+    </row>
+    <row r="655">
+      <c r="A655" s="9"/>
+    </row>
+    <row r="656">
+      <c r="A656" s="9"/>
+    </row>
+    <row r="657">
+      <c r="A657" s="9"/>
+    </row>
+    <row r="658">
+      <c r="A658" s="9"/>
+    </row>
+    <row r="659">
+      <c r="A659" s="9"/>
+    </row>
+    <row r="660">
+      <c r="A660" s="9"/>
+    </row>
+    <row r="661">
+      <c r="A661" s="9"/>
+    </row>
+    <row r="662">
+      <c r="A662" s="9"/>
+    </row>
+    <row r="663">
+      <c r="A663" s="9"/>
+    </row>
+    <row r="664">
+      <c r="A664" s="9"/>
+    </row>
+    <row r="665">
+      <c r="A665" s="9"/>
+    </row>
+    <row r="666">
+      <c r="A666" s="9"/>
+    </row>
+    <row r="667">
+      <c r="A667" s="9"/>
+    </row>
+    <row r="668">
+      <c r="A668" s="9"/>
+    </row>
+    <row r="669">
+      <c r="A669" s="9"/>
+    </row>
+    <row r="670">
+      <c r="A670" s="9"/>
+    </row>
+    <row r="671">
+      <c r="A671" s="9"/>
+    </row>
+    <row r="672">
+      <c r="A672" s="9"/>
+    </row>
+    <row r="673">
+      <c r="A673" s="9"/>
+    </row>
+    <row r="674">
+      <c r="A674" s="9"/>
+    </row>
+    <row r="675">
+      <c r="A675" s="9"/>
+    </row>
+    <row r="676">
+      <c r="A676" s="9"/>
+    </row>
+    <row r="677">
+      <c r="A677" s="9"/>
+    </row>
+    <row r="678">
+      <c r="A678" s="9"/>
+    </row>
+    <row r="679">
+      <c r="A679" s="9"/>
+    </row>
+    <row r="680">
+      <c r="A680" s="9"/>
+    </row>
+    <row r="681">
+      <c r="A681" s="9"/>
+    </row>
+    <row r="682">
+      <c r="A682" s="9"/>
+    </row>
+    <row r="683">
+      <c r="A683" s="9"/>
+    </row>
+    <row r="684">
+      <c r="A684" s="9"/>
+    </row>
+    <row r="685">
+      <c r="A685" s="9"/>
+    </row>
+    <row r="686">
+      <c r="A686" s="9"/>
+    </row>
+    <row r="687">
+      <c r="A687" s="9"/>
+    </row>
+    <row r="688">
+      <c r="A688" s="9"/>
+    </row>
+    <row r="689">
+      <c r="A689" s="9"/>
+    </row>
+    <row r="690">
+      <c r="A690" s="9"/>
+    </row>
+    <row r="691">
+      <c r="A691" s="9"/>
+    </row>
+    <row r="692">
+      <c r="A692" s="9"/>
+    </row>
+    <row r="693">
+      <c r="A693" s="9"/>
+    </row>
+    <row r="694">
+      <c r="A694" s="9"/>
+    </row>
+    <row r="695">
+      <c r="A695" s="9"/>
+    </row>
+    <row r="696">
+      <c r="A696" s="9"/>
+    </row>
+    <row r="697">
+      <c r="A697" s="9"/>
+    </row>
+    <row r="698">
+      <c r="A698" s="9"/>
+    </row>
+    <row r="699">
+      <c r="A699" s="9"/>
+    </row>
+    <row r="700">
+      <c r="A700" s="9"/>
+    </row>
+    <row r="701">
+      <c r="A701" s="9"/>
+    </row>
+    <row r="702">
+      <c r="A702" s="9"/>
+    </row>
+    <row r="703">
+      <c r="A703" s="9"/>
+    </row>
+    <row r="704">
+      <c r="A704" s="9"/>
+    </row>
+    <row r="705">
+      <c r="A705" s="9"/>
+    </row>
+    <row r="706">
+      <c r="A706" s="9"/>
+    </row>
+    <row r="707">
+      <c r="A707" s="9"/>
+    </row>
+    <row r="708">
+      <c r="A708" s="9"/>
+    </row>
+    <row r="709">
+      <c r="A709" s="9"/>
+    </row>
+    <row r="710">
+      <c r="A710" s="9"/>
+    </row>
+    <row r="711">
+      <c r="A711" s="9"/>
+    </row>
+    <row r="712">
+      <c r="A712" s="9"/>
+    </row>
+    <row r="713">
+      <c r="A713" s="9"/>
+    </row>
+    <row r="714">
+      <c r="A714" s="9"/>
+    </row>
+    <row r="715">
+      <c r="A715" s="9"/>
+    </row>
+    <row r="716">
+      <c r="A716" s="9"/>
+    </row>
+    <row r="717">
+      <c r="A717" s="9"/>
+    </row>
+    <row r="718">
+      <c r="A718" s="9"/>
+    </row>
+    <row r="719">
+      <c r="A719" s="9"/>
+    </row>
+    <row r="720">
+      <c r="A720" s="9"/>
+    </row>
+    <row r="721">
+      <c r="A721" s="9"/>
+    </row>
+    <row r="722">
+      <c r="A722" s="9"/>
+    </row>
+    <row r="723">
+      <c r="A723" s="9"/>
+    </row>
+    <row r="724">
+      <c r="A724" s="9"/>
+    </row>
+    <row r="725">
+      <c r="A725" s="9"/>
+    </row>
+    <row r="726">
+      <c r="A726" s="9"/>
+    </row>
+    <row r="727">
+      <c r="A727" s="9"/>
+    </row>
+    <row r="728">
+      <c r="A728" s="9"/>
+    </row>
+    <row r="729">
+      <c r="A729" s="9"/>
+    </row>
+    <row r="730">
+      <c r="A730" s="9"/>
+    </row>
+    <row r="731">
+      <c r="A731" s="9"/>
+    </row>
+    <row r="732">
+      <c r="A732" s="9"/>
+    </row>
+    <row r="733">
+      <c r="A733" s="9"/>
+    </row>
+    <row r="734">
+      <c r="A734" s="9"/>
+    </row>
+    <row r="735">
+      <c r="A735" s="9"/>
+    </row>
+    <row r="736">
+      <c r="A736" s="9"/>
+    </row>
+    <row r="737">
+      <c r="A737" s="9"/>
+    </row>
+    <row r="738">
+      <c r="A738" s="9"/>
+    </row>
+    <row r="739">
+      <c r="A739" s="9"/>
+    </row>
+    <row r="740">
+      <c r="A740" s="9"/>
+    </row>
+    <row r="741">
+      <c r="A741" s="9"/>
+    </row>
+    <row r="742">
+      <c r="A742" s="9"/>
+    </row>
+    <row r="743">
+      <c r="A743" s="9"/>
+    </row>
+    <row r="744">
+      <c r="A744" s="9"/>
+    </row>
+    <row r="745">
+      <c r="A745" s="9"/>
+    </row>
+    <row r="746">
+      <c r="A746" s="9"/>
+    </row>
+    <row r="747">
+      <c r="A747" s="9"/>
+    </row>
+    <row r="748">
+      <c r="A748" s="9"/>
+    </row>
+    <row r="749">
+      <c r="A749" s="9"/>
+    </row>
+    <row r="750">
+      <c r="A750" s="9"/>
+    </row>
+    <row r="751">
+      <c r="A751" s="9"/>
+    </row>
+    <row r="752">
+      <c r="A752" s="9"/>
+    </row>
+    <row r="753">
+      <c r="A753" s="9"/>
+    </row>
+    <row r="754">
+      <c r="A754" s="9"/>
+    </row>
+    <row r="755">
+      <c r="A755" s="9"/>
+    </row>
+    <row r="756">
+      <c r="A756" s="9"/>
+    </row>
+    <row r="757">
+      <c r="A757" s="9"/>
+    </row>
+    <row r="758">
+      <c r="A758" s="9"/>
+    </row>
+    <row r="759">
+      <c r="A759" s="9"/>
+    </row>
+    <row r="760">
+      <c r="A760" s="9"/>
+    </row>
+    <row r="761">
+      <c r="A761" s="9"/>
+    </row>
+    <row r="762">
+      <c r="A762" s="9"/>
+    </row>
+    <row r="763">
+      <c r="A763" s="9"/>
+    </row>
+    <row r="764">
+      <c r="A764" s="9"/>
+    </row>
+    <row r="765">
+      <c r="A765" s="9"/>
+    </row>
+    <row r="766">
+      <c r="A766" s="9"/>
+    </row>
+    <row r="767">
+      <c r="A767" s="9"/>
+    </row>
+    <row r="768">
+      <c r="A768" s="9"/>
+    </row>
+    <row r="769">
+      <c r="A769" s="9"/>
+    </row>
+    <row r="770">
+      <c r="A770" s="9"/>
+    </row>
+    <row r="771">
+      <c r="A771" s="9"/>
+    </row>
+    <row r="772">
+      <c r="A772" s="9"/>
+    </row>
+    <row r="773">
+      <c r="A773" s="9"/>
+    </row>
+    <row r="774">
+      <c r="A774" s="9"/>
+    </row>
+    <row r="775">
+      <c r="A775" s="9"/>
+    </row>
+    <row r="776">
+      <c r="A776" s="9"/>
+    </row>
+    <row r="777">
+      <c r="A777" s="9"/>
+    </row>
+    <row r="778">
+      <c r="A778" s="9"/>
+    </row>
+    <row r="779">
+      <c r="A779" s="9"/>
+    </row>
+    <row r="780">
+      <c r="A780" s="9"/>
+    </row>
+    <row r="781">
+      <c r="A781" s="9"/>
+    </row>
+    <row r="782">
+      <c r="A782" s="9"/>
+    </row>
+    <row r="783">
+      <c r="A783" s="9"/>
+    </row>
+    <row r="784">
+      <c r="A784" s="9"/>
+    </row>
+    <row r="785">
+      <c r="A785" s="9"/>
+    </row>
+    <row r="786">
+      <c r="A786" s="9"/>
+    </row>
+    <row r="787">
+      <c r="A787" s="9"/>
+    </row>
+    <row r="788">
+      <c r="A788" s="9"/>
+    </row>
+    <row r="789">
+      <c r="A789" s="9"/>
+    </row>
+    <row r="790">
+      <c r="A790" s="9"/>
+    </row>
+    <row r="791">
+      <c r="A791" s="9"/>
+    </row>
+    <row r="792">
+      <c r="A792" s="9"/>
+    </row>
+    <row r="793">
+      <c r="A793" s="9"/>
+    </row>
+    <row r="794">
+      <c r="A794" s="9"/>
+    </row>
+    <row r="795">
+      <c r="A795" s="9"/>
+    </row>
+    <row r="796">
+      <c r="A796" s="9"/>
+    </row>
+    <row r="797">
+      <c r="A797" s="9"/>
+    </row>
+    <row r="798">
+      <c r="A798" s="9"/>
+    </row>
+    <row r="799">
+      <c r="A799" s="9"/>
+    </row>
+    <row r="800">
+      <c r="A800" s="9"/>
+    </row>
+    <row r="801">
+      <c r="A801" s="9"/>
+    </row>
+    <row r="802">
+      <c r="A802" s="9"/>
+    </row>
+    <row r="803">
+      <c r="A803" s="9"/>
+    </row>
+    <row r="804">
+      <c r="A804" s="9"/>
+    </row>
+    <row r="805">
+      <c r="A805" s="9"/>
+    </row>
+    <row r="806">
+      <c r="A806" s="9"/>
+    </row>
+    <row r="807">
+      <c r="A807" s="9"/>
+    </row>
+    <row r="808">
+      <c r="A808" s="9"/>
+    </row>
+    <row r="809">
+      <c r="A809" s="9"/>
+    </row>
+    <row r="810">
+      <c r="A810" s="9"/>
+    </row>
+    <row r="811">
+      <c r="A811" s="9"/>
+    </row>
+    <row r="812">
+      <c r="A812" s="9"/>
+    </row>
+    <row r="813">
+      <c r="A813" s="9"/>
+    </row>
+    <row r="814">
+      <c r="A814" s="9"/>
+    </row>
+    <row r="815">
+      <c r="A815" s="9"/>
+    </row>
+    <row r="816">
+      <c r="A816" s="9"/>
+    </row>
+    <row r="817">
+      <c r="A817" s="9"/>
+    </row>
+    <row r="818">
+      <c r="A818" s="9"/>
+    </row>
+    <row r="819">
+      <c r="A819" s="9"/>
+    </row>
+    <row r="820">
+      <c r="A820" s="9"/>
+    </row>
+    <row r="821">
+      <c r="A821" s="9"/>
+    </row>
+    <row r="822">
+      <c r="A822" s="9"/>
+    </row>
+    <row r="823">
+      <c r="A823" s="9"/>
+    </row>
+    <row r="824">
+      <c r="A824" s="9"/>
+    </row>
+    <row r="825">
+      <c r="A825" s="9"/>
+    </row>
+    <row r="826">
+      <c r="A826" s="9"/>
+    </row>
+    <row r="827">
+      <c r="A827" s="9"/>
+    </row>
+    <row r="828">
+      <c r="A828" s="9"/>
+    </row>
+    <row r="829">
+      <c r="A829" s="9"/>
+    </row>
+    <row r="830">
+      <c r="A830" s="9"/>
+    </row>
+    <row r="831">
+      <c r="A831" s="9"/>
+    </row>
+    <row r="832">
+      <c r="A832" s="9"/>
+    </row>
+    <row r="833">
+      <c r="A833" s="9"/>
+    </row>
+    <row r="834">
+      <c r="A834" s="9"/>
+    </row>
+    <row r="835">
+      <c r="A835" s="9"/>
+    </row>
+    <row r="836">
+      <c r="A836" s="9"/>
+    </row>
+    <row r="837">
+      <c r="A837" s="9"/>
+    </row>
+    <row r="838">
+      <c r="A838" s="9"/>
+    </row>
+    <row r="839">
+      <c r="A839" s="9"/>
+    </row>
+    <row r="840">
+      <c r="A840" s="9"/>
+    </row>
+    <row r="841">
+      <c r="A841" s="9"/>
+    </row>
+    <row r="842">
+      <c r="A842" s="9"/>
+    </row>
+    <row r="843">
+      <c r="A843" s="9"/>
+    </row>
+    <row r="844">
+      <c r="A844" s="9"/>
+    </row>
+    <row r="845">
+      <c r="A845" s="9"/>
+    </row>
+    <row r="846">
+      <c r="A846" s="9"/>
+    </row>
+    <row r="847">
+      <c r="A847" s="9"/>
+    </row>
+    <row r="848">
+      <c r="A848" s="9"/>
+    </row>
+    <row r="849">
+      <c r="A849" s="9"/>
+    </row>
+    <row r="850">
+      <c r="A850" s="9"/>
+    </row>
+    <row r="851">
+      <c r="A851" s="9"/>
+    </row>
+    <row r="852">
+      <c r="A852" s="9"/>
+    </row>
+    <row r="853">
+      <c r="A853" s="9"/>
+    </row>
+    <row r="854">
+      <c r="A854" s="9"/>
+    </row>
+    <row r="855">
+      <c r="A855" s="9"/>
+    </row>
+    <row r="856">
+      <c r="A856" s="9"/>
+    </row>
+    <row r="857">
+      <c r="A857" s="9"/>
+    </row>
+    <row r="858">
+      <c r="A858" s="9"/>
+    </row>
+    <row r="859">
+      <c r="A859" s="9"/>
+    </row>
+    <row r="860">
+      <c r="A860" s="9"/>
+    </row>
+    <row r="861">
+      <c r="A861" s="9"/>
+    </row>
+    <row r="862">
+      <c r="A862" s="9"/>
+    </row>
+    <row r="863">
+      <c r="A863" s="9"/>
+    </row>
+    <row r="864">
+      <c r="A864" s="9"/>
+    </row>
+    <row r="865">
+      <c r="A865" s="9"/>
+    </row>
+    <row r="866">
+      <c r="A866" s="9"/>
+    </row>
+    <row r="867">
+      <c r="A867" s="9"/>
+    </row>
+    <row r="868">
+      <c r="A868" s="9"/>
+    </row>
+    <row r="869">
+      <c r="A869" s="9"/>
+    </row>
+    <row r="870">
+      <c r="A870" s="9"/>
+    </row>
+    <row r="871">
+      <c r="A871" s="9"/>
+    </row>
+    <row r="872">
+      <c r="A872" s="9"/>
+    </row>
+    <row r="873">
+      <c r="A873" s="9"/>
+    </row>
+    <row r="874">
+      <c r="A874" s="9"/>
+    </row>
+    <row r="875">
+      <c r="A875" s="9"/>
+    </row>
+    <row r="876">
+      <c r="A876" s="9"/>
+    </row>
+    <row r="877">
+      <c r="A877" s="9"/>
+    </row>
+    <row r="878">
+      <c r="A878" s="9"/>
+    </row>
+    <row r="879">
+      <c r="A879" s="9"/>
+    </row>
+    <row r="880">
+      <c r="A880" s="9"/>
+    </row>
+    <row r="881">
+      <c r="A881" s="9"/>
+    </row>
+    <row r="882">
+      <c r="A882" s="9"/>
+    </row>
+    <row r="883">
+      <c r="A883" s="9"/>
+    </row>
+    <row r="884">
+      <c r="A884" s="9"/>
+    </row>
+    <row r="885">
+      <c r="A885" s="9"/>
+    </row>
+    <row r="886">
+      <c r="A886" s="9"/>
+    </row>
+    <row r="887">
+      <c r="A887" s="9"/>
+    </row>
+    <row r="888">
+      <c r="A888" s="9"/>
+    </row>
+    <row r="889">
+      <c r="A889" s="9"/>
+    </row>
+    <row r="890">
+      <c r="A890" s="9"/>
+    </row>
+    <row r="891">
+      <c r="A891" s="9"/>
+    </row>
+    <row r="892">
+      <c r="A892" s="9"/>
+    </row>
+    <row r="893">
+      <c r="A893" s="9"/>
+    </row>
+    <row r="894">
+      <c r="A894" s="9"/>
+    </row>
+    <row r="895">
+      <c r="A895" s="9"/>
+    </row>
+    <row r="896">
+      <c r="A896" s="9"/>
+    </row>
+    <row r="897">
+      <c r="A897" s="9"/>
+    </row>
+    <row r="898">
+      <c r="A898" s="9"/>
+    </row>
+    <row r="899">
+      <c r="A899" s="9"/>
+    </row>
+    <row r="900">
+      <c r="A900" s="9"/>
+    </row>
+    <row r="901">
+      <c r="A901" s="9"/>
+    </row>
+    <row r="902">
+      <c r="A902" s="9"/>
+    </row>
+    <row r="903">
+      <c r="A903" s="9"/>
+    </row>
+    <row r="904">
+      <c r="A904" s="9"/>
+    </row>
+    <row r="905">
+      <c r="A905" s="9"/>
+    </row>
+    <row r="906">
+      <c r="A906" s="9"/>
+    </row>
+    <row r="907">
+      <c r="A907" s="9"/>
+    </row>
+    <row r="908">
+      <c r="A908" s="9"/>
+    </row>
+    <row r="909">
+      <c r="A909" s="9"/>
+    </row>
+    <row r="910">
+      <c r="A910" s="9"/>
+    </row>
+    <row r="911">
+      <c r="A911" s="9"/>
+    </row>
+    <row r="912">
+      <c r="A912" s="9"/>
+    </row>
+    <row r="913">
+      <c r="A913" s="9"/>
+    </row>
+    <row r="914">
+      <c r="A914" s="9"/>
+    </row>
+    <row r="915">
+      <c r="A915" s="9"/>
+    </row>
+    <row r="916">
+      <c r="A916" s="9"/>
+    </row>
+    <row r="917">
+      <c r="A917" s="9"/>
+    </row>
+    <row r="918">
+      <c r="A918" s="9"/>
+    </row>
+    <row r="919">
+      <c r="A919" s="9"/>
+    </row>
+    <row r="920">
+      <c r="A920" s="9"/>
+    </row>
+    <row r="921">
+      <c r="A921" s="9"/>
+    </row>
+    <row r="922">
+      <c r="A922" s="9"/>
+    </row>
+    <row r="923">
+      <c r="A923" s="9"/>
+    </row>
+    <row r="924">
+      <c r="A924" s="9"/>
+    </row>
+    <row r="925">
+      <c r="A925" s="9"/>
+    </row>
+    <row r="926">
+      <c r="A926" s="9"/>
+    </row>
+    <row r="927">
+      <c r="A927" s="9"/>
+    </row>
+    <row r="928">
+      <c r="A928" s="9"/>
+    </row>
+    <row r="929">
+      <c r="A929" s="9"/>
+    </row>
+    <row r="930">
+      <c r="A930" s="9"/>
+    </row>
+    <row r="931">
+      <c r="A931" s="9"/>
+    </row>
+    <row r="932">
+      <c r="A932" s="9"/>
+    </row>
+    <row r="933">
+      <c r="A933" s="9"/>
+    </row>
+    <row r="934">
+      <c r="A934" s="9"/>
+    </row>
+    <row r="935">
+      <c r="A935" s="9"/>
+    </row>
+    <row r="936">
+      <c r="A936" s="9"/>
+    </row>
+    <row r="937">
+      <c r="A937" s="9"/>
+    </row>
+    <row r="938">
+      <c r="A938" s="9"/>
+    </row>
+    <row r="939">
+      <c r="A939" s="9"/>
+    </row>
+    <row r="940">
+      <c r="A940" s="9"/>
+    </row>
+    <row r="941">
+      <c r="A941" s="9"/>
+    </row>
+    <row r="942">
+      <c r="A942" s="9"/>
+    </row>
+    <row r="943">
+      <c r="A943" s="9"/>
+    </row>
+    <row r="944">
+      <c r="A944" s="9"/>
+    </row>
+    <row r="945">
+      <c r="A945" s="9"/>
+    </row>
+    <row r="946">
+      <c r="A946" s="9"/>
+    </row>
+    <row r="947">
+      <c r="A947" s="9"/>
+    </row>
+    <row r="948">
+      <c r="A948" s="9"/>
+    </row>
+    <row r="949">
+      <c r="A949" s="9"/>
+    </row>
+    <row r="950">
+      <c r="A950" s="9"/>
+    </row>
+    <row r="951">
+      <c r="A951" s="9"/>
+    </row>
+    <row r="952">
+      <c r="A952" s="9"/>
+    </row>
+    <row r="953">
+      <c r="A953" s="9"/>
+    </row>
+    <row r="954">
+      <c r="A954" s="9"/>
+    </row>
+    <row r="955">
+      <c r="A955" s="9"/>
+    </row>
+    <row r="956">
+      <c r="A956" s="9"/>
+    </row>
+    <row r="957">
+      <c r="A957" s="9"/>
+    </row>
+    <row r="958">
+      <c r="A958" s="9"/>
+    </row>
+    <row r="959">
+      <c r="A959" s="9"/>
+    </row>
+    <row r="960">
+      <c r="A960" s="9"/>
+    </row>
+    <row r="961">
+      <c r="A961" s="9"/>
+    </row>
+    <row r="962">
+      <c r="A962" s="9"/>
+    </row>
+    <row r="963">
+      <c r="A963" s="9"/>
+    </row>
+    <row r="964">
+      <c r="A964" s="9"/>
+    </row>
+    <row r="965">
+      <c r="A965" s="9"/>
+    </row>
+    <row r="966">
+      <c r="A966" s="9"/>
+    </row>
+    <row r="967">
+      <c r="A967" s="9"/>
+    </row>
+    <row r="968">
+      <c r="A968" s="9"/>
+    </row>
+    <row r="969">
+      <c r="A969" s="9"/>
+    </row>
+    <row r="970">
+      <c r="A970" s="9"/>
+    </row>
+    <row r="971">
+      <c r="A971" s="9"/>
+    </row>
+    <row r="972">
+      <c r="A972" s="9"/>
+    </row>
+    <row r="973">
+      <c r="A973" s="9"/>
+    </row>
+    <row r="974">
+      <c r="A974" s="9"/>
+    </row>
+    <row r="975">
+      <c r="A975" s="9"/>
+    </row>
+    <row r="976">
+      <c r="A976" s="9"/>
+    </row>
+    <row r="977">
+      <c r="A977" s="9"/>
+    </row>
+    <row r="978">
+      <c r="A978" s="9"/>
+    </row>
+    <row r="979">
+      <c r="A979" s="9"/>
+    </row>
+    <row r="980">
+      <c r="A980" s="9"/>
+    </row>
+    <row r="981">
+      <c r="A981" s="9"/>
+    </row>
+    <row r="982">
+      <c r="A982" s="9"/>
+    </row>
+    <row r="983">
+      <c r="A983" s="9"/>
+    </row>
+    <row r="984">
+      <c r="A984" s="9"/>
+    </row>
+    <row r="985">
+      <c r="A985" s="9"/>
+    </row>
+    <row r="986">
+      <c r="A986" s="9"/>
+    </row>
+    <row r="987">
+      <c r="A987" s="9"/>
+    </row>
+    <row r="988">
+      <c r="A988" s="9"/>
+    </row>
+    <row r="989">
+      <c r="A989" s="9"/>
+    </row>
+    <row r="990">
+      <c r="A990" s="9"/>
+    </row>
+    <row r="991">
+      <c r="A991" s="9"/>
+    </row>
+    <row r="992">
+      <c r="A992" s="9"/>
+    </row>
+    <row r="993">
+      <c r="A993" s="9"/>
+    </row>
+    <row r="994">
+      <c r="A994" s="9"/>
+    </row>
+    <row r="995">
+      <c r="A995" s="9"/>
+    </row>
+    <row r="996">
+      <c r="A996" s="9"/>
+    </row>
+    <row r="997">
+      <c r="A997" s="9"/>
+    </row>
+    <row r="998">
+      <c r="A998" s="9"/>
+    </row>
+    <row r="999">
+      <c r="A999" s="9"/>
+    </row>
+    <row r="1000">
+      <c r="A1000" s="9"/>
+    </row>
+  </sheetData>
+  <dataValidations>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A1000">
+      <formula1>OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D"))</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D2"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
iniciando a integracao do selenium com beautifulsoap
</commit_message>
<xml_diff>
--- a/assets/base_dados.xlsx
+++ b/assets/base_dados.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="10">
   <si>
     <t>data</t>
   </si>
@@ -889,9 +889,15 @@
       <c r="A15" s="6">
         <v>45189.0</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="B15" s="7">
+        <v>0.5416666666666666</v>
+      </c>
+      <c r="C15" s="8">
+        <v>95.9</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1036,7 +1042,9 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="1"/>
+      <c r="A20" s="6">
+        <v>45194.0</v>
+      </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1064,7 +1072,9 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="1"/>
+      <c r="A21" s="6">
+        <v>45195.0</v>
+      </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1092,7 +1102,9 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="1"/>
+      <c r="A22" s="6">
+        <v>45196.0</v>
+      </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1120,7 +1132,9 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="1"/>
+      <c r="A23" s="6">
+        <v>45197.0</v>
+      </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1148,7 +1162,9 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="1"/>
+      <c r="A24" s="6">
+        <v>45198.0</v>
+      </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1176,7 +1192,9 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="1"/>
+      <c r="A25" s="6">
+        <v>45199.0</v>
+      </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1204,7 +1222,9 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="1"/>
+      <c r="A26" s="6">
+        <v>45200.0</v>
+      </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1232,7 +1252,9 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="1"/>
+      <c r="A27" s="6">
+        <v>45201.0</v>
+      </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1260,7 +1282,9 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="1"/>
+      <c r="A28" s="6">
+        <v>45202.0</v>
+      </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1288,7 +1312,9 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="1"/>
+      <c r="A29" s="6">
+        <v>45203.0</v>
+      </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1316,7 +1342,9 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="1"/>
+      <c r="A30" s="6">
+        <v>45204.0</v>
+      </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1344,7 +1372,9 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="1"/>
+      <c r="A31" s="6">
+        <v>45205.0</v>
+      </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1372,7 +1402,9 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="1"/>
+      <c r="A32" s="6">
+        <v>45206.0</v>
+      </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1400,7 +1432,9 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="1"/>
+      <c r="A33" s="6">
+        <v>45207.0</v>
+      </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1428,7 +1462,9 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="1"/>
+      <c r="A34" s="6">
+        <v>45208.0</v>
+      </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1456,7 +1492,9 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="1"/>
+      <c r="A35" s="6">
+        <v>45209.0</v>
+      </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1484,7 +1522,9 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="1"/>
+      <c r="A36" s="6">
+        <v>45210.0</v>
+      </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -1512,7 +1552,9 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="1"/>
+      <c r="A37" s="6">
+        <v>45211.0</v>
+      </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1540,7 +1582,9 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="1"/>
+      <c r="A38" s="6">
+        <v>45212.0</v>
+      </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1568,7 +1612,9 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="1"/>
+      <c r="A39" s="6">
+        <v>45213.0</v>
+      </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1596,7 +1642,9 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="1"/>
+      <c r="A40" s="6">
+        <v>45214.0</v>
+      </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -28960,6 +29008,12 @@
       <c r="A26" s="14">
         <v>45189.0</v>
       </c>
+      <c r="B26" s="15">
+        <v>0.5416666666666666</v>
+      </c>
+      <c r="C26" s="10">
+        <v>2817.0</v>
+      </c>
       <c r="D26" s="13" t="s">
         <v>6</v>
       </c>
@@ -28970,6 +29024,12 @@
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="14">
         <v>45189.0</v>
+      </c>
+      <c r="B27" s="15">
+        <v>0.5416666666666666</v>
+      </c>
+      <c r="C27" s="10">
+        <v>2468.0</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>8</v>
@@ -28982,6 +29042,12 @@
       <c r="A28" s="14">
         <v>45189.0</v>
       </c>
+      <c r="B28" s="15">
+        <v>0.5416666666666666</v>
+      </c>
+      <c r="C28" s="10">
+        <v>0.0</v>
+      </c>
       <c r="D28" s="10" t="s">
         <v>6</v>
       </c>
@@ -28989,9 +29055,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1">
+      <c r="A29" s="14">
+        <v>45190.0</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25" customHeight="1">
+      <c r="A30" s="14">
+        <v>45190.0</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25" customHeight="1">
+      <c r="A31" s="14">
+        <v>45190.0</v>
+      </c>
+    </row>
     <row r="32" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
@@ -30063,6 +30141,18 @@
       <c r="A5" s="17">
         <v>45189.0</v>
       </c>
+      <c r="B5" s="15">
+        <v>0.5416666666666666</v>
+      </c>
+      <c r="C5" s="10">
+        <v>2270.0</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="17">

</xml_diff>

<commit_message>
correcao do erro de click para buscar na pagina
</commit_message>
<xml_diff>
--- a/assets/base_dados.xlsx
+++ b/assets/base_dados.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="10">
   <si>
     <t>data</t>
   </si>
@@ -925,9 +925,15 @@
       <c r="A16" s="6">
         <v>45190.0</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="B16" s="7">
+        <v>0.8229166666666666</v>
+      </c>
+      <c r="C16" s="8">
+        <v>95.9</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -29059,15 +29065,51 @@
       <c r="A29" s="14">
         <v>45190.0</v>
       </c>
+      <c r="B29" s="15">
+        <v>0.8229166666666666</v>
+      </c>
+      <c r="C29" s="10">
+        <v>2584.0</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="14">
         <v>45190.0</v>
       </c>
+      <c r="B30" s="15">
+        <v>0.8229166666666666</v>
+      </c>
+      <c r="C30" s="10">
+        <v>2468.0</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="14">
         <v>45190.0</v>
+      </c>
+      <c r="B31" s="15">
+        <v>0.8229166666666666</v>
+      </c>
+      <c r="C31" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1"/>
@@ -30051,11 +30093,12 @@
     <hyperlink r:id="rId8" ref="D20"/>
     <hyperlink r:id="rId9" ref="D23"/>
     <hyperlink r:id="rId10" ref="D26"/>
+    <hyperlink r:id="rId11" ref="D29"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.787401575" footer="0.0" header="0.0" left="0.511811024" right="0.511811024" top="0.787401575"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId11"/>
+  <drawing r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -30158,6 +30201,18 @@
       <c r="A6" s="17">
         <v>45190.0</v>
       </c>
+      <c r="B6" s="15">
+        <v>0.8229166666666666</v>
+      </c>
+      <c r="C6" s="10">
+        <v>2285.0</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="17">

</xml_diff>